<commit_message>
Adding Problems With Solutions ( Update Repo)
</commit_message>
<xml_diff>
--- a/List of  the problems.xlsx
+++ b/List of  the problems.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakar\Desktop\Project 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakar\OneDrive\Desktop\Problem_solving-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6478D3FC-8283-404D-B765-62C6091E1F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122F0CC7-A2D6-4FB1-B9FB-78E232A55133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="34">
   <si>
     <t>Problem Name</t>
   </si>
@@ -115,13 +115,25 @@
   </si>
   <si>
     <t>Minutes Before the New Year</t>
+  </si>
+  <si>
+    <t>Beautiful Matrix</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/contest/263/problem/A</t>
+  </si>
+  <si>
+    <t>Gravity Flip</t>
+  </si>
+  <si>
+    <t>http://codeforces.com/contest/405/problem/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +183,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -199,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -211,6 +235,8 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -569,7 +595,7 @@
   <dimension ref="D1:F152"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,15 +891,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="4:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+    <row r="27" spans="4:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="D27" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="28" spans="4:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="D28" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="29" spans="4:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="D29" s="3"/>
@@ -1527,11 +1565,12 @@
     <hyperlink ref="E24" r:id="rId28" display="https://codeforces.com/contest/520/problem/A" xr:uid="{1F44DFAD-58B5-40BA-8BB6-798B97E37FA9}"/>
     <hyperlink ref="E25" r:id="rId29" display="https://codeforces.com/contest/443/problem/A" xr:uid="{8F7742DD-CABC-4170-99E3-9426F07EE3F3}"/>
     <hyperlink ref="E26" r:id="rId30" display="https://codeforces.com/contest/1283/problem/A" xr:uid="{D4EF6C67-C015-4AA8-A23A-BED1F7EEE0A2}"/>
+    <hyperlink ref="E27" r:id="rId31" xr:uid="{5BD48735-EE33-4213-9E01-A258A62062F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
   <tableParts count="1">
-    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId33"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Repo by Adding Problems
</commit_message>
<xml_diff>
--- a/List of  the problems.xlsx
+++ b/List of  the problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakar\OneDrive\Desktop\Problem_solving-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122F0CC7-A2D6-4FB1-B9FB-78E232A55133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D731A88-BC97-44C8-96B4-4BE15FA65584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
   <si>
     <t>Problem Name</t>
   </si>
@@ -127,13 +127,37 @@
   </si>
   <si>
     <t>http://codeforces.com/contest/405/problem/A</t>
+  </si>
+  <si>
+    <t>Magnets</t>
+  </si>
+  <si>
+    <t>http://codeforces.com/contest/344/problem/A</t>
+  </si>
+  <si>
+    <t>Sereja and Dima</t>
+  </si>
+  <si>
+    <t>http://codeforces.com/contest/381/problem/A</t>
+  </si>
+  <si>
+    <t>Police Recruits</t>
+  </si>
+  <si>
+    <t>Black Square</t>
+  </si>
+  <si>
+    <t>http://codeforces.com/contest/427/problem/A</t>
+  </si>
+  <si>
+    <t>http://codeforces.com/contest/431/problem/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +219,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Bell MT"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -223,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -237,6 +267,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -594,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268EC9E1-576B-4D3E-9533-8F1EB4DB00EC}">
   <dimension ref="D1:F152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,25 +944,49 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="4:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="4:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+    <row r="29" spans="4:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="D29" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="D30" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="31" spans="4:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="D31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="32" spans="4:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="D32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="33" spans="4:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="D33" s="3"/>
@@ -1566,11 +1621,15 @@
     <hyperlink ref="E25" r:id="rId29" display="https://codeforces.com/contest/443/problem/A" xr:uid="{8F7742DD-CABC-4170-99E3-9426F07EE3F3}"/>
     <hyperlink ref="E26" r:id="rId30" display="https://codeforces.com/contest/1283/problem/A" xr:uid="{D4EF6C67-C015-4AA8-A23A-BED1F7EEE0A2}"/>
     <hyperlink ref="E27" r:id="rId31" xr:uid="{5BD48735-EE33-4213-9E01-A258A62062F4}"/>
+    <hyperlink ref="E29" r:id="rId32" xr:uid="{37C2E17F-3F80-41F2-835B-F942659B1379}"/>
+    <hyperlink ref="E30" r:id="rId33" xr:uid="{4440FBFF-53B2-45CC-8123-3785DEBD7BEC}"/>
+    <hyperlink ref="E31" r:id="rId34" xr:uid="{8B81643F-DFCF-4467-983B-9B29EE26AD83}"/>
+    <hyperlink ref="E32" r:id="rId35" xr:uid="{B55D4EBE-8330-458D-AE23-458814309627}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
   <tableParts count="1">
-    <tablePart r:id="rId33"/>
+    <tablePart r:id="rId37"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>